<commit_message>
add header to menus
</commit_message>
<xml_diff>
--- a/src/main/resources/JobDistribution.xlsx
+++ b/src/main/resources/JobDistribution.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aryan\IdeaProjects\Project_team-34\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sharif\Project_team-34(clone number 85)\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6F1E09-6EBA-41F3-8204-26786A519A18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{EE7FFC58-2647-46D7-803F-1059478E6AD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="GUI" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -135,7 +134,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -210,7 +209,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -225,7 +223,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -240,7 +237,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -255,7 +251,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Consolas"/>
-        <family val="3"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -270,7 +265,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -285,7 +279,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -303,22 +296,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2910FFAF-71CC-4809-B649-47122B60F999}" name="Table2" displayName="Table2" ref="A1:C29" headerRowCount="0" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C29" headerRowCount="0" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{7E9F9D8C-623B-4D1C-9C4A-D5B7BCB460AC}" name="Column1" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{4F679F2F-2E48-4C35-A960-BA20A90C42C2}" name="Column2" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{FF98C18F-8527-4947-97E7-FA1A734A6346}" name="Column3" headerRowDxfId="2" dataDxfId="1"/>
+    <tableColumn id="1" name="Column1" dataDxfId="4"/>
+    <tableColumn id="2" name="Column2" dataDxfId="3"/>
+    <tableColumn id="3" name="Column3" headerRowDxfId="2" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A7260EA6-9A1A-4D63-A930-37A9F4346B06}" name="Table3" displayName="Table3" ref="E14:G16" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="E14:G16" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6C5DBE57-75BA-4F2B-9043-BD1EC87452A0}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{AB4F6C0B-77E8-4E2B-A235-E8A798A0C625}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{40DAB3B4-DE35-4844-9CF6-113F91677E11}" name="Column3" dataDxfId="0"/>
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -620,23 +613,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3313C0BA-EC2D-4B6C-B0FC-36269D3C108E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="6" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="40.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.44140625" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="6" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -647,7 +640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -655,10 +648,10 @@
         <v>24</v>
       </c>
       <c r="C2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -666,10 +659,10 @@
         <v>24</v>
       </c>
       <c r="C3" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -680,7 +673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -691,7 +684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -699,10 +692,10 @@
         <v>24</v>
       </c>
       <c r="C6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -713,7 +706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -724,7 +717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -732,10 +725,10 @@
         <v>24</v>
       </c>
       <c r="C9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -746,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -757,7 +750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -768,7 +761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -776,10 +769,10 @@
         <v>24</v>
       </c>
       <c r="C13" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -797,7 +790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -815,7 +808,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -833,7 +826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -844,7 +837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
@@ -855,7 +848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
@@ -866,7 +859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -874,10 +867,10 @@
         <v>24</v>
       </c>
       <c r="C20" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
@@ -888,7 +881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
@@ -899,7 +892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -907,10 +900,10 @@
         <v>24</v>
       </c>
       <c r="C23" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>31</v>
       </c>
@@ -918,10 +911,10 @@
         <v>24</v>
       </c>
       <c r="C24" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
@@ -932,7 +925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
@@ -943,7 +936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -951,10 +944,10 @@
         <v>24</v>
       </c>
       <c r="C27" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
@@ -965,7 +958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Add Category related Menus
</commit_message>
<xml_diff>
--- a/src/main/resources/JobDistribution.xlsx
+++ b/src/main/resources/JobDistribution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aryan\Project_team-34\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764F89F1-B5EE-4225-8E55-E4ECF0C9D550}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE24A57C-B9FA-49D6-BDD0-08B48BE9ACA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -660,7 +660,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,11 +849,11 @@
       </c>
       <c r="G14">
         <f>COUNTIFS(C:C, 1, B:B, Table3[[#This Row],[Persooon]])</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H14">
         <f>Table3[[#This Row],[Total]]-Table3[[#This Row],[Dones]]</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1048,7 +1048,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>